<commit_message>
fix last name issue in fellows
</commit_message>
<xml_diff>
--- a/csv/selected_aspirants.xlsx
+++ b/csv/selected_aspirants.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Macbamba\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Macbamba\Proyectos\PHP\agentes-v2\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>emails</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>saguilar@egesac.org</t>
-  </si>
-  <si>
-    <t>teredolz@cotaipec.org.mx</t>
   </si>
   <si>
     <t>thelma.beltran@gmail.com</t>
@@ -464,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,11 +669,6 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>